<commit_message>
correcting data, and updating graph
</commit_message>
<xml_diff>
--- a/Looking_into_PremierLeague_2016-17/Teams/Crystal_Palace.xlsx
+++ b/Looking_into_PremierLeague_2016-17/Teams/Crystal_Palace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BFCFC5-5F48-40DF-9000-FD76E5864863}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398CAB4A-01C4-4B1A-B096-234F2C358440}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="151">
   <si>
     <t>Arsenal</t>
   </si>
@@ -70,12 +70,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>GER</t>
-  </si>
-  <si>
-    <t>Werder Bremen</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -184,139 +178,7 @@
     <t>Hednesford T</t>
   </si>
   <si>
-    <t>Players no longer at this club</t>
-  </si>
-  <si>
-    <t>New Club</t>
-  </si>
-  <si>
-    <t>Tafari Moore</t>
-  </si>
-  <si>
-    <t>Brent</t>
-  </si>
-  <si>
-    <t>FC Utrecht (On Loan)</t>
-  </si>
-  <si>
-    <t>Joel Campbell</t>
-  </si>
-  <si>
-    <t>CRC</t>
-  </si>
-  <si>
-    <t>San José [CRC]</t>
-  </si>
-  <si>
-    <t>Sporting CP (On Loan)</t>
-  </si>
-  <si>
-    <t>Calum Chambers</t>
-  </si>
-  <si>
-    <t>Petersfield</t>
-  </si>
-  <si>
-    <t>Middlesbrough (On Loan)</t>
-  </si>
-  <si>
-    <t>Jack Wilshere</t>
-  </si>
-  <si>
-    <t>Stevenage</t>
-  </si>
-  <si>
-    <t>Bournemouth (On Loan)</t>
-  </si>
-  <si>
-    <t>Serge Gnabry</t>
-  </si>
-  <si>
-    <t>Stuttgart</t>
-  </si>
-  <si>
-    <t>Chuba Akpom</t>
-  </si>
-  <si>
-    <t>Newham</t>
-  </si>
-  <si>
-    <t>Brighton &amp; HA (On Loan)</t>
-  </si>
-  <si>
-    <t>Ismaël Bennacer</t>
-  </si>
-  <si>
-    <t>ALG</t>
-  </si>
-  <si>
-    <t>Arles</t>
-  </si>
-  <si>
-    <t>Tours (On Loan)</t>
-  </si>
-  <si>
-    <t>Krystian Bielik</t>
-  </si>
-  <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>Konin</t>
-  </si>
-  <si>
-    <t>Birmingham C (On Loan)</t>
-  </si>
-  <si>
-    <t>Marc Bola</t>
-  </si>
-  <si>
-    <t>Notts Co (On Loan)</t>
-  </si>
-  <si>
-    <t>Gedion Zelalem</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>VVV Venlo (On Loan)</t>
-  </si>
-  <si>
-    <t>Aaron Eyoma</t>
-  </si>
-  <si>
-    <t>Hackney</t>
-  </si>
-  <si>
-    <t>FC Volendam (On Loan)</t>
-  </si>
-  <si>
-    <t>Kaylen Hinds</t>
-  </si>
-  <si>
-    <t>Stevenage (On Loan)</t>
-  </si>
-  <si>
-    <t>Stephy Mavididi</t>
-  </si>
-  <si>
-    <t>Derby</t>
-  </si>
-  <si>
-    <t>Charlton Ath (On Loan)</t>
-  </si>
-  <si>
-    <t>Tyrell Robinson</t>
-  </si>
-  <si>
     <t>Basildon</t>
-  </si>
-  <si>
-    <t>Nathan Tella</t>
   </si>
   <si>
     <t>IRL</t>
@@ -1107,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I52"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,19 +981,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="96" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:9" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="G3"/>
     </row>
@@ -1172,13 +1034,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="13">
         <v>1.86</v>
@@ -1190,10 +1052,10 @@
         <v>28993</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1201,7 +1063,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>13</v>
@@ -1219,10 +1081,10 @@
         <v>32810</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1230,10 +1092,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>11</v>
@@ -1248,10 +1110,10 @@
         <v>33114</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1259,13 +1121,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>120</v>
+        <v>74</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" s="13">
         <v>1.78</v>
@@ -1277,7 +1139,7 @@
         <v>30748</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>0</v>
@@ -1288,7 +1150,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>13</v>
@@ -1306,10 +1168,10 @@
         <v>32596</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1317,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>123</v>
+        <v>77</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>13</v>
@@ -1335,10 +1197,10 @@
         <v>31822</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1346,13 +1208,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="13">
         <v>1.74</v>
@@ -1364,10 +1226,10 @@
         <v>31426</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1375,13 +1237,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="16">
         <v>1.84</v>
@@ -1393,10 +1255,10 @@
         <v>31779</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1404,13 +1266,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="13">
         <v>1.72</v>
@@ -1422,10 +1284,10 @@
         <v>32033</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1433,13 +1295,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15" s="13">
         <v>1.81</v>
@@ -1451,7 +1313,7 @@
         <v>33435</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>12</v>
@@ -1462,13 +1324,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16" s="13">
         <v>1.8</v>
@@ -1480,10 +1342,10 @@
         <v>33918</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1491,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>10</v>
@@ -1509,10 +1371,10 @@
         <v>32917</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1520,13 +1382,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="C18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="E18" s="13">
         <v>1.97</v>
@@ -1538,10 +1400,10 @@
         <v>31801</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1549,13 +1411,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E19" s="13">
         <v>1.8</v>
@@ -1567,10 +1429,10 @@
         <v>32326</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1578,13 +1440,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" s="13">
         <v>1.86</v>
@@ -1596,10 +1458,10 @@
         <v>34817</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1607,13 +1469,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="13">
         <v>1.83</v>
@@ -1625,10 +1487,10 @@
         <v>31800</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1636,13 +1498,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" s="13">
         <v>1.9</v>
@@ -1654,10 +1516,10 @@
         <v>33210</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1665,13 +1527,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E23" s="13">
         <v>1.78</v>
@@ -1683,10 +1545,10 @@
         <v>32057</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1694,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>13</v>
@@ -1712,10 +1574,10 @@
         <v>33856</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1736,13 +1598,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="13">
         <v>1.89</v>
@@ -1754,10 +1616,10 @@
         <v>34059</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1778,10 +1640,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>11</v>
@@ -1796,10 +1658,10 @@
         <v>33030</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1820,13 +1682,13 @@
         <v>25</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E30" s="13">
         <v>1.82</v>
@@ -1838,7 +1700,7 @@
         <v>34937</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>15</v>
@@ -1849,13 +1711,13 @@
         <v>26</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E31" s="13">
         <v>1.84</v>
@@ -1867,10 +1729,10 @@
         <v>32257</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1878,10 +1740,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>11</v>
@@ -1896,10 +1758,10 @@
         <v>29796</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1907,13 +1769,13 @@
         <v>28</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E33" s="13">
         <v>1.83</v>
@@ -1925,10 +1787,10 @@
         <v>33335</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1949,13 +1811,13 @@
         <v>30</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E35" s="13">
         <v>1.85</v>
@@ -1967,10 +1829,10 @@
         <v>31134</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1978,13 +1840,13 @@
         <v>31</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>176</v>
+        <v>130</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E36" s="13">
         <v>1.78</v>
@@ -1996,10 +1858,10 @@
         <v>33961</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>177</v>
+        <v>131</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>178</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2033,7 +1895,7 @@
         <v>34</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>13</v>
@@ -2051,10 +1913,10 @@
         <v>32990</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2062,13 +1924,13 @@
         <v>35</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E40" s="13">
         <v>1.83</v>
@@ -2080,7 +1942,7 @@
         <v>36126</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>15</v>
@@ -2143,13 +2005,13 @@
         <v>40</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E45" s="13">
         <v>1.88</v>
@@ -2161,10 +2023,10 @@
         <v>34707</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2172,13 +2034,13 @@
         <v>42</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E46" s="13">
         <v>1.73</v>
@@ -2190,10 +2052,10 @@
         <v>31589</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2201,7 +2063,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>13</v>
@@ -2219,7 +2081,7 @@
         <v>35775</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
       <c r="I47" s="12" t="s">
         <v>15</v>
@@ -2230,13 +2092,13 @@
         <v>45</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E48" s="13">
         <v>1.74</v>
@@ -2248,7 +2110,7 @@
         <v>35695</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I48" s="12" t="s">
         <v>15</v>
@@ -2259,13 +2121,13 @@
         <v>46</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>191</v>
+        <v>145</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E49" s="13">
         <v>1.83</v>
@@ -2277,7 +2139,7 @@
         <v>35760</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
       <c r="I49" s="12" t="s">
         <v>15</v>
@@ -2288,13 +2150,13 @@
         <v>47</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -2302,7 +2164,7 @@
         <v>35749</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I50" s="12" t="s">
         <v>15</v>
@@ -2313,13 +2175,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E51" s="13">
         <v>1.73</v>
@@ -2331,10 +2193,10 @@
         <v>36556</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2342,13 +2204,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
@@ -2356,7 +2218,7 @@
         <v>36455</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>196</v>
+        <v>150</v>
       </c>
       <c r="I52" s="12" t="s">
         <v>15</v>
@@ -2422,13 +2284,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E58" s="4">
         <v>1.77</v>
@@ -2440,7 +2302,7 @@
         <v>35671</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>15</v>
@@ -2451,13 +2313,13 @@
         <v>56</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E59" s="4">
         <v>1.76</v>
@@ -2469,10 +2331,10 @@
         <v>36169</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2480,13 +2342,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2494,7 +2356,7 @@
         <v>36193</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>15</v>
@@ -2505,13 +2367,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -2519,7 +2381,7 @@
         <v>35870</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>15</v>
@@ -2530,7 +2392,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>13</v>
@@ -2544,10 +2406,10 @@
         <v>36070</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2555,13 +2417,13 @@
         <v>65</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E63" s="4">
         <v>1.85</v>
@@ -2573,10 +2435,10 @@
         <v>35831</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2584,13 +2446,13 @@
         <v>68</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E64" s="4">
         <v>1.78</v>
@@ -2602,7 +2464,7 @@
         <v>35826</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>15</v>
@@ -2613,13 +2475,13 @@
         <v>72</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E65" s="4">
         <v>1.75</v>
@@ -2642,13 +2504,13 @@
         <v>73</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -2656,7 +2518,7 @@
         <v>36310</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>15</v>
@@ -2667,10 +2529,10 @@
         <v>76</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>11</v>
@@ -2690,13 +2552,13 @@
         <v>82</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -2704,7 +2566,7 @@
         <v>36392</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>15</v>
@@ -2715,7 +2577,7 @@
         <v>85</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>13</v>
@@ -2733,16 +2595,14 @@
         <v>35157</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="18" t="s">
-        <v>54</v>
-      </c>
+      <c r="A70" s="18"/>
       <c r="B70" s="18"/>
       <c r="C70" s="18"/>
       <c r="D70" s="18"/>
@@ -2753,462 +2613,180 @@
       <c r="I70" s="18"/>
     </row>
     <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="3">
-        <v>59</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="4">
-        <v>1.73</v>
-      </c>
-      <c r="F72" s="4">
-        <v>66</v>
-      </c>
-      <c r="G72" s="7">
-        <v>35616</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="3">
-        <v>28</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E73" s="4">
-        <v>1.78</v>
-      </c>
-      <c r="F73" s="4">
-        <v>70</v>
-      </c>
-      <c r="G73" s="7">
-        <v>33781</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="3">
-        <v>21</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" s="4">
-        <v>1.82</v>
-      </c>
-      <c r="F74" s="4">
-        <v>66</v>
-      </c>
-      <c r="G74" s="7">
-        <v>34719</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="3">
-        <v>10</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E75" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="F75" s="4">
-        <v>65</v>
-      </c>
-      <c r="G75" s="7">
-        <v>33604</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="3">
-        <v>27</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E76" s="4">
-        <v>1.73</v>
-      </c>
-      <c r="F76" s="4">
-        <v>73</v>
-      </c>
-      <c r="G76" s="7">
-        <v>34894</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="3">
-        <v>32</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E77" s="4">
-        <v>1.83</v>
-      </c>
-      <c r="F77" s="4">
-        <v>77</v>
-      </c>
-      <c r="G77" s="7">
-        <v>34981</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="3">
-        <v>36</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E78" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="F78" s="4">
-        <v>70</v>
-      </c>
-      <c r="G78" s="7">
-        <v>35765</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="3">
-        <v>37</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E79" s="4">
-        <v>1.89</v>
-      </c>
-      <c r="F79" s="4">
-        <v>78</v>
-      </c>
-      <c r="G79" s="7">
-        <v>35799</v>
-      </c>
-      <c r="H79" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="3">
-        <v>38</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="F80" s="4">
-        <v>78</v>
-      </c>
-      <c r="G80" s="7">
-        <v>35773</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="3">
-        <v>40</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E81" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="F81" s="4">
-        <v>77</v>
-      </c>
-      <c r="G81" s="7">
-        <v>35456</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="3">
-        <v>44</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="F82" s="4">
-        <v>70</v>
-      </c>
-      <c r="G82" s="7">
-        <v>35695</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="3">
-        <v>48</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E83" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="F83" s="4">
-        <v>68</v>
-      </c>
-      <c r="G83" s="7">
-        <v>35823</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="3">
-        <v>57</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E84" s="4">
-        <v>1.82</v>
-      </c>
-      <c r="F84" s="4">
-        <v>71</v>
-      </c>
-      <c r="G84" s="7">
-        <v>35946</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="3">
-        <v>64</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E85" s="4">
-        <v>1.73</v>
-      </c>
-      <c r="F85" s="4">
-        <v>68</v>
-      </c>
-      <c r="G85" s="7">
-        <v>35689</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+    </row>
+    <row r="84" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+    </row>
+    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="3"/>
       <c r="I85" s="3"/>
     </row>
-    <row r="86" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3">
-        <v>78</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>20</v>
-      </c>
+    <row r="86" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="7">
-        <v>36346</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="G86" s="7"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>